<commit_message>
next commit rest rest
</commit_message>
<xml_diff>
--- a/src/test/resources/Restaurant.xlsx
+++ b/src/test/resources/Restaurant.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -68,6 +68,12 @@
     <t>Point of Contact Phone Number</t>
   </si>
   <si>
+    <t>Sales Manager</t>
+  </si>
+  <si>
+    <t>Restaurant Category</t>
+  </si>
+  <si>
     <t>draftland testing 1</t>
   </si>
   <si>
@@ -102,6 +108,9 @@
   </si>
   <si>
     <t>6512 3333</t>
+  </si>
+  <si>
+    <t>John</t>
   </si>
 </sst>
 </file>
@@ -717,7 +726,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1037,10 +1046,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -1059,9 +1068,10 @@
     <col min="12" max="12" width="16.5714285714286" customWidth="1"/>
     <col min="13" max="13" width="32" customWidth="1"/>
     <col min="14" max="14" width="14.4285714285714" customWidth="1"/>
+    <col min="15" max="15" width="20.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1101,46 +1111,58 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E2">
         <v>654512</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="M2" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="N2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit updates 2 restaurant
</commit_message>
<xml_diff>
--- a/src/test/resources/Restaurant.xlsx
+++ b/src/test/resources/Restaurant.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -74,6 +74,12 @@
     <t>Restaurant Category</t>
   </si>
   <si>
+    <t>Platform Account</t>
+  </si>
+  <si>
+    <t>Connect Account</t>
+  </si>
+  <si>
     <t>draftland testing 1</t>
   </si>
   <si>
@@ -111,6 +117,12 @@
   </si>
   <si>
     <t>John</t>
+  </si>
+  <si>
+    <t>EatMe - POS 2 (acct_1O9kwUAaoVAZ6m8M)</t>
+  </si>
+  <si>
+    <t>acct_1REm1MPMERGGWtpY</t>
   </si>
 </sst>
 </file>
@@ -1046,10 +1058,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -1069,9 +1081,11 @@
     <col min="13" max="13" width="32" customWidth="1"/>
     <col min="14" max="14" width="14.4285714285714" customWidth="1"/>
     <col min="15" max="15" width="20.5714285714286" customWidth="1"/>
+    <col min="16" max="16" width="32" customWidth="1"/>
+    <col min="17" max="17" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1117,52 +1131,64 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E2">
         <v>654512</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="M2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="O2">
         <v>2</v>
+      </c>
+      <c r="P2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>